<commit_message>
Exceloperations data files added
</commit_message>
<xml_diff>
--- a/seleniumProject/src/test/java/excelDataDriven/testdata1.xlsx
+++ b/seleniumProject/src/test/java/excelDataDriven/testdata1.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>UserName</t>
   </si>
@@ -90,13 +90,30 @@
   </si>
   <si>
     <t>Passed</t>
+  </si>
+  <si>
+    <t>Aborted</t>
+  </si>
+  <si>
+    <t>TestCase Name</t>
+  </si>
+  <si>
+    <t>TC-1</t>
+  </si>
+  <si>
+    <t>TC-2</t>
+  </si>
+  <si>
+    <t>TC-3</t>
+  </si>
+  <si>
+    <t>TC-4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -492,17 +509,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -552,7 +569,9 @@
       <c r="D3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
@@ -594,12 +613,75 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>